<commit_message>
recognition_table unified with encoding and updated
</commit_message>
<xml_diff>
--- a/StimuliTable-Recognition_3-runs_40-pairs_8-discrete-loc_12345-delays.xlsx
+++ b/StimuliTable-Recognition_3-runs_40-pairs_8-discrete-loc_12345-delays.xlsx
@@ -245,7 +245,7 @@
   <dimension ref="A1:AMJ145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:I1"/>
+      <selection pane="topLeft" activeCell="B181" activeCellId="0" sqref="B146:B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -360,6 +360,9 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
@@ -377,6 +380,9 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
@@ -394,6 +400,9 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
@@ -411,6 +420,9 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
@@ -428,6 +440,9 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
@@ -445,6 +460,9 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
@@ -462,6 +480,9 @@
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
@@ -479,6 +500,9 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
@@ -496,6 +520,9 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
@@ -513,6 +540,9 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
@@ -530,6 +560,9 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>6000</v>
+      </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
@@ -547,6 +580,9 @@
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
@@ -564,6 +600,9 @@
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
       </c>
@@ -581,6 +620,9 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
@@ -598,6 +640,9 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="B16" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
@@ -615,6 +660,9 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
@@ -632,6 +680,9 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
       </c>
@@ -649,6 +700,9 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
@@ -666,6 +720,9 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B20" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D20" s="0" t="n">
         <v>2</v>
       </c>
@@ -683,6 +740,9 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D21" s="0" t="n">
         <v>2</v>
       </c>
@@ -700,6 +760,9 @@
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D22" s="0" t="n">
         <v>2</v>
       </c>
@@ -717,6 +780,9 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D23" s="0" t="n">
         <v>2</v>
       </c>
@@ -734,6 +800,9 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
@@ -751,6 +820,9 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D25" s="0" t="n">
         <v>2</v>
       </c>
@@ -768,6 +840,9 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D26" s="0" t="n">
         <v>2</v>
       </c>
@@ -785,6 +860,9 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D27" s="0" t="n">
         <v>2</v>
       </c>
@@ -802,6 +880,9 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D28" s="0" t="n">
         <v>2</v>
       </c>
@@ -819,6 +900,9 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D29" s="0" t="n">
         <v>2</v>
       </c>
@@ -836,6 +920,9 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D30" s="0" t="n">
         <v>2</v>
       </c>
@@ -853,6 +940,9 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <v>8000</v>
+      </c>
       <c r="D31" s="0" t="n">
         <v>2</v>
       </c>
@@ -870,6 +960,9 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D32" s="0" t="n">
         <v>2</v>
       </c>
@@ -886,6 +979,9 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>500</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>2</v>
@@ -904,6 +1000,9 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D34" s="0" t="n">
         <v>2</v>
       </c>
@@ -921,6 +1020,9 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D35" s="0" t="n">
         <v>2</v>
       </c>
@@ -938,6 +1040,9 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D36" s="0" t="n">
         <v>2</v>
       </c>
@@ -955,6 +1060,9 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D37" s="0" t="n">
         <v>2</v>
       </c>
@@ -972,6 +1080,9 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D38" s="0" t="n">
         <v>3</v>
       </c>
@@ -989,6 +1100,9 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D39" s="0" t="n">
         <v>3</v>
       </c>
@@ -1006,6 +1120,9 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="n">
+        <v>6000</v>
+      </c>
       <c r="D40" s="0" t="n">
         <v>3</v>
       </c>
@@ -1023,6 +1140,9 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D41" s="0" t="n">
         <v>3</v>
       </c>
@@ -1040,6 +1160,9 @@
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D42" s="0" t="n">
         <v>3</v>
       </c>
@@ -1057,6 +1180,9 @@
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D43" s="0" t="n">
         <v>3</v>
       </c>
@@ -1074,6 +1200,9 @@
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="B44" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D44" s="0" t="n">
         <v>3</v>
       </c>
@@ -1091,6 +1220,9 @@
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="B45" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D45" s="0" t="n">
         <v>3</v>
       </c>
@@ -1108,6 +1240,9 @@
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="B46" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D46" s="0" t="n">
         <v>3</v>
       </c>
@@ -1125,6 +1260,9 @@
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="B47" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D47" s="0" t="n">
         <v>3</v>
       </c>
@@ -1142,6 +1280,9 @@
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="B48" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D48" s="0" t="n">
         <v>3</v>
       </c>
@@ -1159,6 +1300,9 @@
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="B49" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D49" s="0" t="n">
         <v>3</v>
       </c>
@@ -1176,6 +1320,9 @@
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="B50" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D50" s="0" t="n">
         <v>3</v>
       </c>
@@ -1193,6 +1340,9 @@
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B51" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D51" s="0" t="n">
         <v>3</v>
       </c>
@@ -1210,6 +1360,9 @@
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="B52" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D52" s="0" t="n">
         <v>3</v>
       </c>
@@ -1227,6 +1380,9 @@
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="B53" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D53" s="0" t="n">
         <v>3</v>
       </c>
@@ -1244,6 +1400,9 @@
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="B54" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D54" s="0" t="n">
         <v>3</v>
       </c>
@@ -1261,6 +1420,9 @@
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
+      <c r="B55" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D55" s="0" t="n">
         <v>3</v>
       </c>
@@ -1278,6 +1440,9 @@
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="B56" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D56" s="0" t="n">
         <v>4</v>
       </c>
@@ -1295,6 +1460,9 @@
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="B57" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D57" s="0" t="n">
         <v>4</v>
       </c>
@@ -1312,6 +1480,9 @@
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="B58" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D58" s="0" t="n">
         <v>4</v>
       </c>
@@ -1329,6 +1500,9 @@
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="B59" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D59" s="0" t="n">
         <v>4</v>
       </c>
@@ -1346,6 +1520,9 @@
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="B60" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D60" s="0" t="n">
         <v>4</v>
       </c>
@@ -1363,6 +1540,9 @@
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="B61" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D61" s="0" t="n">
         <v>4</v>
       </c>
@@ -1380,6 +1560,9 @@
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
+      <c r="B62" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D62" s="0" t="n">
         <v>4</v>
       </c>
@@ -1397,6 +1580,9 @@
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="B63" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D63" s="0" t="n">
         <v>4</v>
       </c>
@@ -1414,6 +1600,9 @@
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="B64" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
       </c>
@@ -1431,6 +1620,9 @@
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="B65" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D65" s="0" t="n">
         <v>4</v>
       </c>
@@ -1448,6 +1640,9 @@
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="B66" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D66" s="0" t="n">
         <v>4</v>
       </c>
@@ -1465,6 +1660,9 @@
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="B67" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D67" s="0" t="n">
         <v>4</v>
       </c>
@@ -1482,6 +1680,9 @@
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
+      <c r="B68" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D68" s="0" t="n">
         <v>4</v>
       </c>
@@ -1499,6 +1700,9 @@
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
+      <c r="B69" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D69" s="0" t="n">
         <v>4</v>
       </c>
@@ -1516,6 +1720,9 @@
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="B70" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D70" s="0" t="n">
         <v>4</v>
       </c>
@@ -1533,6 +1740,9 @@
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="B71" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D71" s="0" t="n">
         <v>4</v>
       </c>
@@ -1550,6 +1760,9 @@
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="B72" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D72" s="0" t="n">
         <v>4</v>
       </c>
@@ -1567,6 +1780,9 @@
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="B73" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D73" s="0" t="n">
         <v>4</v>
       </c>
@@ -1584,6 +1800,9 @@
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
+      <c r="B74" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D74" s="0" t="n">
         <v>5</v>
       </c>
@@ -1601,6 +1820,9 @@
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="B75" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D75" s="0" t="n">
         <v>5</v>
       </c>
@@ -1618,6 +1840,9 @@
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="B76" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D76" s="0" t="n">
         <v>5</v>
       </c>
@@ -1635,6 +1860,9 @@
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D77" s="0" t="n">
         <v>5</v>
       </c>
@@ -1652,6 +1880,9 @@
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="B78" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D78" s="0" t="n">
         <v>5</v>
       </c>
@@ -1669,6 +1900,9 @@
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="B79" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D79" s="0" t="n">
         <v>5</v>
       </c>
@@ -1686,6 +1920,9 @@
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="B80" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D80" s="0" t="n">
         <v>5</v>
       </c>
@@ -1703,6 +1940,9 @@
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="B81" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D81" s="0" t="n">
         <v>5</v>
       </c>
@@ -1720,6 +1960,9 @@
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
+      <c r="B82" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D82" s="0" t="n">
         <v>5</v>
       </c>
@@ -1737,6 +1980,9 @@
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
+      <c r="B83" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D83" s="0" t="n">
         <v>5</v>
       </c>
@@ -1754,6 +2000,9 @@
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
+      <c r="B84" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D84" s="0" t="n">
         <v>5</v>
       </c>
@@ -1771,6 +2020,9 @@
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
+      <c r="B85" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D85" s="0" t="n">
         <v>5</v>
       </c>
@@ -1788,6 +2040,9 @@
       <c r="A86" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="B86" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D86" s="0" t="n">
         <v>5</v>
       </c>
@@ -1805,6 +2060,9 @@
       <c r="A87" s="0" t="n">
         <v>86</v>
       </c>
+      <c r="B87" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D87" s="0" t="n">
         <v>5</v>
       </c>
@@ -1822,6 +2080,9 @@
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
+      <c r="B88" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D88" s="0" t="n">
         <v>5</v>
       </c>
@@ -1839,6 +2100,9 @@
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="B89" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D89" s="0" t="n">
         <v>5</v>
       </c>
@@ -1856,6 +2120,9 @@
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="B90" s="0" t="n">
+        <v>8000</v>
+      </c>
       <c r="D90" s="0" t="n">
         <v>5</v>
       </c>
@@ -1873,6 +2140,9 @@
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="B91" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D91" s="0" t="n">
         <v>5</v>
       </c>
@@ -1890,6 +2160,9 @@
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="B92" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D92" s="0" t="n">
         <v>6</v>
       </c>
@@ -1907,6 +2180,9 @@
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
+      <c r="B93" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D93" s="0" t="n">
         <v>6</v>
       </c>
@@ -1924,6 +2200,9 @@
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="B94" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D94" s="0" t="n">
         <v>6</v>
       </c>
@@ -1941,6 +2220,9 @@
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="B95" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D95" s="0" t="n">
         <v>6</v>
       </c>
@@ -1958,6 +2240,9 @@
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="B96" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D96" s="0" t="n">
         <v>6</v>
       </c>
@@ -1975,6 +2260,9 @@
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="B97" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D97" s="0" t="n">
         <v>6</v>
       </c>
@@ -1992,6 +2280,9 @@
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
+      <c r="B98" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D98" s="0" t="n">
         <v>6</v>
       </c>
@@ -2009,6 +2300,9 @@
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
+      <c r="B99" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D99" s="0" t="n">
         <v>6</v>
       </c>
@@ -2026,6 +2320,9 @@
       <c r="A100" s="0" t="n">
         <v>99</v>
       </c>
+      <c r="B100" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D100" s="0" t="n">
         <v>6</v>
       </c>
@@ -2043,6 +2340,9 @@
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B101" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D101" s="0" t="n">
         <v>6</v>
       </c>
@@ -2060,6 +2360,9 @@
       <c r="A102" s="0" t="n">
         <v>101</v>
       </c>
+      <c r="B102" s="0" t="n">
+        <v>8000</v>
+      </c>
       <c r="D102" s="0" t="n">
         <v>6</v>
       </c>
@@ -2077,6 +2380,9 @@
       <c r="A103" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="B103" s="0" t="n">
+        <v>6000</v>
+      </c>
       <c r="D103" s="0" t="n">
         <v>6</v>
       </c>
@@ -2094,6 +2400,9 @@
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
+      <c r="B104" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D104" s="0" t="n">
         <v>6</v>
       </c>
@@ -2111,6 +2420,9 @@
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="B105" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D105" s="0" t="n">
         <v>6</v>
       </c>
@@ -2128,6 +2440,9 @@
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
+      <c r="B106" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D106" s="0" t="n">
         <v>6</v>
       </c>
@@ -2145,6 +2460,9 @@
       <c r="A107" s="0" t="n">
         <v>106</v>
       </c>
+      <c r="B107" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D107" s="0" t="n">
         <v>6</v>
       </c>
@@ -2162,6 +2480,9 @@
       <c r="A108" s="0" t="n">
         <v>107</v>
       </c>
+      <c r="B108" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D108" s="0" t="n">
         <v>6</v>
       </c>
@@ -2179,6 +2500,9 @@
       <c r="A109" s="0" t="n">
         <v>108</v>
       </c>
+      <c r="B109" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D109" s="0" t="n">
         <v>6</v>
       </c>
@@ -2196,6 +2520,9 @@
       <c r="A110" s="0" t="n">
         <v>109</v>
       </c>
+      <c r="B110" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D110" s="0" t="n">
         <v>7</v>
       </c>
@@ -2213,6 +2540,9 @@
       <c r="A111" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="B111" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D111" s="0" t="n">
         <v>7</v>
       </c>
@@ -2230,6 +2560,9 @@
       <c r="A112" s="0" t="n">
         <v>111</v>
       </c>
+      <c r="B112" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D112" s="0" t="n">
         <v>7</v>
       </c>
@@ -2247,6 +2580,9 @@
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="B113" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D113" s="0" t="n">
         <v>7</v>
       </c>
@@ -2264,6 +2600,9 @@
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
+      <c r="B114" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D114" s="0" t="n">
         <v>7</v>
       </c>
@@ -2281,6 +2620,9 @@
       <c r="A115" s="0" t="n">
         <v>114</v>
       </c>
+      <c r="B115" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D115" s="0" t="n">
         <v>7</v>
       </c>
@@ -2298,6 +2640,9 @@
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
+      <c r="B116" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D116" s="0" t="n">
         <v>7</v>
       </c>
@@ -2315,6 +2660,9 @@
       <c r="A117" s="0" t="n">
         <v>116</v>
       </c>
+      <c r="B117" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D117" s="0" t="n">
         <v>7</v>
       </c>
@@ -2332,6 +2680,9 @@
       <c r="A118" s="0" t="n">
         <v>117</v>
       </c>
+      <c r="B118" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D118" s="0" t="n">
         <v>7</v>
       </c>
@@ -2349,6 +2700,9 @@
       <c r="A119" s="0" t="n">
         <v>118</v>
       </c>
+      <c r="B119" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D119" s="0" t="n">
         <v>7</v>
       </c>
@@ -2366,6 +2720,9 @@
       <c r="A120" s="0" t="n">
         <v>119</v>
       </c>
+      <c r="B120" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D120" s="0" t="n">
         <v>7</v>
       </c>
@@ -2383,6 +2740,9 @@
       <c r="A121" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="B121" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D121" s="0" t="n">
         <v>7</v>
       </c>
@@ -2400,6 +2760,9 @@
       <c r="A122" s="0" t="n">
         <v>121</v>
       </c>
+      <c r="B122" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D122" s="0" t="n">
         <v>7</v>
       </c>
@@ -2417,6 +2780,9 @@
       <c r="A123" s="0" t="n">
         <v>122</v>
       </c>
+      <c r="B123" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D123" s="0" t="n">
         <v>7</v>
       </c>
@@ -2434,6 +2800,9 @@
       <c r="A124" s="0" t="n">
         <v>123</v>
       </c>
+      <c r="B124" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D124" s="0" t="n">
         <v>7</v>
       </c>
@@ -2451,6 +2820,9 @@
       <c r="A125" s="0" t="n">
         <v>124</v>
       </c>
+      <c r="B125" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D125" s="0" t="n">
         <v>7</v>
       </c>
@@ -2468,6 +2840,9 @@
       <c r="A126" s="0" t="n">
         <v>125</v>
       </c>
+      <c r="B126" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D126" s="0" t="n">
         <v>7</v>
       </c>
@@ -2485,6 +2860,9 @@
       <c r="A127" s="0" t="n">
         <v>126</v>
       </c>
+      <c r="B127" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D127" s="0" t="n">
         <v>7</v>
       </c>
@@ -2502,6 +2880,9 @@
       <c r="A128" s="0" t="n">
         <v>127</v>
       </c>
+      <c r="B128" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D128" s="0" t="n">
         <v>8</v>
       </c>
@@ -2519,6 +2900,9 @@
       <c r="A129" s="0" t="n">
         <v>128</v>
       </c>
+      <c r="B129" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D129" s="0" t="n">
         <v>8</v>
       </c>
@@ -2536,6 +2920,9 @@
       <c r="A130" s="0" t="n">
         <v>129</v>
       </c>
+      <c r="B130" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D130" s="0" t="n">
         <v>8</v>
       </c>
@@ -2553,6 +2940,9 @@
       <c r="A131" s="0" t="n">
         <v>130</v>
       </c>
+      <c r="B131" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D131" s="0" t="n">
         <v>8</v>
       </c>
@@ -2570,6 +2960,9 @@
       <c r="A132" s="0" t="n">
         <v>131</v>
       </c>
+      <c r="B132" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D132" s="0" t="n">
         <v>8</v>
       </c>
@@ -2587,6 +2980,9 @@
       <c r="A133" s="0" t="n">
         <v>132</v>
       </c>
+      <c r="B133" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D133" s="0" t="n">
         <v>8</v>
       </c>
@@ -2604,6 +3000,9 @@
       <c r="A134" s="0" t="n">
         <v>133</v>
       </c>
+      <c r="B134" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D134" s="0" t="n">
         <v>8</v>
       </c>
@@ -2621,6 +3020,9 @@
       <c r="A135" s="0" t="n">
         <v>134</v>
       </c>
+      <c r="B135" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D135" s="0" t="n">
         <v>8</v>
       </c>
@@ -2638,6 +3040,9 @@
       <c r="A136" s="0" t="n">
         <v>135</v>
       </c>
+      <c r="B136" s="0" t="n">
+        <v>4000</v>
+      </c>
       <c r="D136" s="0" t="n">
         <v>8</v>
       </c>
@@ -2655,6 +3060,9 @@
       <c r="A137" s="0" t="n">
         <v>136</v>
       </c>
+      <c r="B137" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D137" s="0" t="n">
         <v>8</v>
       </c>
@@ -2672,6 +3080,9 @@
       <c r="A138" s="0" t="n">
         <v>137</v>
       </c>
+      <c r="B138" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D138" s="0" t="n">
         <v>8</v>
       </c>
@@ -2689,6 +3100,9 @@
       <c r="A139" s="0" t="n">
         <v>138</v>
       </c>
+      <c r="B139" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D139" s="0" t="n">
         <v>8</v>
       </c>
@@ -2706,6 +3120,9 @@
       <c r="A140" s="0" t="n">
         <v>139</v>
       </c>
+      <c r="B140" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="D140" s="0" t="n">
         <v>8</v>
       </c>
@@ -2723,6 +3140,9 @@
       <c r="A141" s="0" t="n">
         <v>140</v>
       </c>
+      <c r="B141" s="0" t="n">
+        <v>500</v>
+      </c>
       <c r="D141" s="0" t="n">
         <v>8</v>
       </c>
@@ -2740,6 +3160,9 @@
       <c r="A142" s="0" t="n">
         <v>141</v>
       </c>
+      <c r="B142" s="0" t="n">
+        <v>5000</v>
+      </c>
       <c r="D142" s="0" t="n">
         <v>8</v>
       </c>
@@ -2757,6 +3180,9 @@
       <c r="A143" s="0" t="n">
         <v>142</v>
       </c>
+      <c r="B143" s="0" t="n">
+        <v>2000</v>
+      </c>
       <c r="D143" s="0" t="n">
         <v>8</v>
       </c>
@@ -2774,6 +3200,9 @@
       <c r="A144" s="0" t="n">
         <v>143</v>
       </c>
+      <c r="B144" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="D144" s="0" t="n">
         <v>8</v>
       </c>
@@ -2790,6 +3219,9 @@
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
         <v>144</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>500</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>8</v>

</xml_diff>